<commit_message>
new updates required by HQ
</commit_message>
<xml_diff>
--- a/output/summary_sorted/summary_sorted_2018_covid.xlsx
+++ b/output/summary_sorted/summary_sorted_2018_covid.xlsx
@@ -241,13 +241,13 @@
     <t>categorical</t>
   </si>
   <si>
-    <t>0.606462611916377</t>
-  </si>
-  <si>
-    <t>0.579333867947464</t>
-  </si>
-  <si>
-    <t>0.63359135588529</t>
+    <t>0.612198042251963</t>
+  </si>
+  <si>
+    <t>0.589417154213208</t>
+  </si>
+  <si>
+    <t>0.634978930290718</t>
   </si>
   <si>
     <t>% HH with "moderately insecure" or "severely insecure" food security status, using CARI Analysis (composite using FCS, food expenditure share, and CS categories)</t>
@@ -256,51 +256,51 @@
     <t>numerical</t>
   </si>
   <si>
-    <t>1.57321545838306</t>
-  </si>
-  <si>
-    <t>1.54449090375351</t>
-  </si>
-  <si>
-    <t>1.6019400130126</t>
+    <t>1.5767011737072</t>
+  </si>
+  <si>
+    <t>1.54818563997836</t>
+  </si>
+  <si>
+    <t>1.60521670743605</t>
   </si>
   <si>
     <t>% of HHs with a poor FCS</t>
   </si>
   <si>
-    <t>0.0227262381036789</t>
-  </si>
-  <si>
-    <t>0.0166586211305778</t>
-  </si>
-  <si>
-    <t>0.02879385507678</t>
+    <t>0.0184992044521441</t>
+  </si>
+  <si>
+    <t>0.0144954913046134</t>
+  </si>
+  <si>
+    <t>0.0225029175996748</t>
   </si>
   <si>
     <t>% HH relying on emergency strategies to cope with a lack of resources to meet basic needs. 
 (also analyse for each of the strategies highlighted in red individually)</t>
   </si>
   <si>
-    <t>0.775682375782498</t>
-  </si>
-  <si>
-    <t>0.75601336521456</t>
-  </si>
-  <si>
-    <t>0.795351386350436</t>
+    <t>0.792974208655268</t>
+  </si>
+  <si>
+    <t>0.777096605921233</t>
+  </si>
+  <si>
+    <t>0.808851811389304</t>
   </si>
   <si>
     <t>% of HH spending more than 40% of their total expenditure on food
 (for 2020 we'd also need the percentages for the following percentage categories: 0%-9.9%, 10%-19.9%, 20%-29.9%......)</t>
   </si>
   <si>
-    <t>0.411276055706418</t>
-  </si>
-  <si>
-    <t>0.388222032928396</t>
-  </si>
-  <si>
-    <t>0.434330078484441</t>
+    <t>0.4004785208465</t>
+  </si>
+  <si>
+    <t>0.381331111201067</t>
+  </si>
+  <si>
+    <t>0.419625930491934</t>
   </si>
   <si>
     <t>Protection</t>
@@ -309,13 +309,13 @@
     <t>% HH with children with psychosocial distress (proxy data with behaviour change)</t>
   </si>
   <si>
-    <t>0.164496953129986</t>
-  </si>
-  <si>
-    <t>0.145338741113525</t>
-  </si>
-  <si>
-    <t>0.183655165146447</t>
+    <t>0.165182141008942</t>
+  </si>
+  <si>
+    <t>0.149092332067627</t>
+  </si>
+  <si>
+    <t>0.181271949950257</t>
   </si>
   <si>
     <t>Livelihoods</t>
@@ -324,109 +324,109 @@
     <t>% HH with at least one adult (18+) unemployed and seeking work</t>
   </si>
   <si>
-    <t>0.293805063110464</t>
-  </si>
-  <si>
-    <t>0.271887175684228</t>
-  </si>
-  <si>
-    <t>0.315722950536701</t>
+    <t>0.300474194695268</t>
+  </si>
+  <si>
+    <t>0.281894165755412</t>
+  </si>
+  <si>
+    <t>0.319054223635123</t>
   </si>
   <si>
     <t>% HH with at least one person under (&lt;18) working</t>
   </si>
   <si>
-    <t>0.168910751225079</t>
-  </si>
-  <si>
-    <t>0.144325357659691</t>
-  </si>
-  <si>
-    <t>0.193496144790466</t>
+    <t>0.176686557319134</t>
+  </si>
+  <si>
+    <t>0.15559833619663</t>
+  </si>
+  <si>
+    <t>0.197774778441638</t>
   </si>
   <si>
     <t>% of female headed households whose average monthly income [from employment and pension] was less than 480,000 IQD/month</t>
   </si>
   <si>
-    <t>0.493716100991197</t>
-  </si>
-  <si>
-    <t>0.354419757478374</t>
-  </si>
-  <si>
-    <t>0.63301244450402</t>
+    <t>0.498508806279197</t>
+  </si>
+  <si>
+    <t>0.380146639476169</t>
+  </si>
+  <si>
+    <t>0.616870973082225</t>
   </si>
   <si>
     <t>% of households relying  on humanitarian assistance as a primary  source of income</t>
   </si>
   <si>
-    <t>0.0127487598203877</t>
-  </si>
-  <si>
-    <t>0.00795597362033751</t>
-  </si>
-  <si>
-    <t>0.0175415460204379</t>
+    <t>0.0124891468867089</t>
+  </si>
+  <si>
+    <t>0.00882919935041235</t>
+  </si>
+  <si>
+    <t>0.0161490944230054</t>
   </si>
   <si>
     <t>% HH with all working adults in unstable employment</t>
   </si>
   <si>
-    <t>0.609634692344655</t>
-  </si>
-  <si>
-    <t>0.583445865898794</t>
-  </si>
-  <si>
-    <t>0.635823518790515</t>
+    <t>0.606183919810635</t>
+  </si>
+  <si>
+    <t>0.584117571528862</t>
+  </si>
+  <si>
+    <t>0.628250268092408</t>
   </si>
   <si>
     <t>% HH spending more than 30% of total expenditure on rent</t>
   </si>
   <si>
-    <t>0.451878736136754</t>
-  </si>
-  <si>
-    <t>0.428104515934778</t>
-  </si>
-  <si>
-    <t>0.475652956338731</t>
+    <t>0.454156531655008</t>
+  </si>
+  <si>
+    <t>0.434187189195005</t>
+  </si>
+  <si>
+    <t>0.47412587411501</t>
   </si>
   <si>
     <t xml:space="preserve">% HH with debt value &gt; 505,000 IQD </t>
   </si>
   <si>
-    <t>0.487992403337838</t>
-  </si>
-  <si>
-    <t>0.464407616306882</t>
-  </si>
-  <si>
-    <t>0.511577190368794</t>
+    <t>0.505566144991947</t>
+  </si>
+  <si>
+    <t>0.485840224253345</t>
+  </si>
+  <si>
+    <t>0.525292065730549</t>
   </si>
   <si>
     <t>% HH unable to afford basic needs (% HH taking on debt due to healthcare, food, education, or basic household expenditures)</t>
   </si>
   <si>
-    <t>0.641119195952551</t>
-  </si>
-  <si>
-    <t>0.618104576143286</t>
-  </si>
-  <si>
-    <t>0.664133815761816</t>
+    <t>0.654143529990814</t>
+  </si>
+  <si>
+    <t>0.635001479690299</t>
+  </si>
+  <si>
+    <t>0.673285580291329</t>
   </si>
   <si>
     <t>% HHs reporting risk of eviction</t>
   </si>
   <si>
-    <t>0.0669238445994565</t>
-  </si>
-  <si>
-    <t>0.0547236776669703</t>
-  </si>
-  <si>
-    <t>0.0791240115319427</t>
+    <t>0.0671147270162204</t>
+  </si>
+  <si>
+    <t>0.0570485508205628</t>
+  </si>
+  <si>
+    <t>0.077180903211878</t>
   </si>
   <si>
     <t>AAP</t>
@@ -435,25 +435,25 @@
     <t xml:space="preserve">% HH reporting to have received aid </t>
   </si>
   <si>
-    <t>0.108329172109907</t>
-  </si>
-  <si>
-    <t>0.0962787173294586</t>
-  </si>
-  <si>
-    <t>0.120379626890356</t>
+    <t>0.100476217626806</t>
+  </si>
+  <si>
+    <t>0.0913989929608189</t>
+  </si>
+  <si>
+    <t>0.109553442292794</t>
   </si>
   <si>
     <t xml:space="preserve">% HH satsified with aid received </t>
   </si>
   <si>
-    <t>0.715385220986666</t>
-  </si>
-  <si>
-    <t>0.666400895122181</t>
-  </si>
-  <si>
-    <t>0.764369546851152</t>
+    <t>0.675840709835964</t>
+  </si>
+  <si>
+    <t>0.6326379428972</t>
+  </si>
+  <si>
+    <t>0.719043476774729</t>
   </si>
   <si>
     <t>% HH not satsified by reason</t>
@@ -463,49 +463,49 @@
 </t>
   </si>
   <si>
-    <t>0.0557398690409635</t>
-  </si>
-  <si>
-    <t>0.0305432809195503</t>
-  </si>
-  <si>
-    <t>0.0809364571623767</t>
+    <t>0.0651079547980969</t>
+  </si>
+  <si>
+    <t>0.0413623380682663</t>
+  </si>
+  <si>
+    <t>0.0888535715279275</t>
   </si>
   <si>
     <t>Quantity not enough</t>
   </si>
   <si>
-    <t>0.183175109817025</t>
-  </si>
-  <si>
-    <t>0.14137087014553</t>
-  </si>
-  <si>
-    <t>0.22497934948852</t>
+    <t>0.207498554885757</t>
+  </si>
+  <si>
+    <t>0.169444100447101</t>
+  </si>
+  <si>
+    <t>0.245553009324412</t>
   </si>
   <si>
     <t>Delays in delivery of aid</t>
   </si>
   <si>
-    <t>0.0265592247065934</t>
-  </si>
-  <si>
-    <t>0.00856201709904261</t>
-  </si>
-  <si>
-    <t>0.0445564323141442</t>
+    <t>0.0297435478031087</t>
+  </si>
+  <si>
+    <t>0.012691752561205</t>
+  </si>
+  <si>
+    <t>0.0467953430450125</t>
   </si>
   <si>
     <t>Other</t>
   </si>
   <si>
-    <t>0.00454305686086231</t>
-  </si>
-  <si>
-    <t>-0.00175540250359762</t>
-  </si>
-  <si>
-    <t>0.0108415162253222</t>
+    <t>0.00612903123352411</t>
+  </si>
+  <si>
+    <t>-0.00112782837659553</t>
+  </si>
+  <si>
+    <t>0.0133858908436437</t>
   </si>
   <si>
     <t>Risk Profile</t>
@@ -515,13 +515,13 @@
 </t>
   </si>
   <si>
-    <t>0.790451797980362</t>
-  </si>
-  <si>
-    <t>0.772541494791014</t>
-  </si>
-  <si>
-    <t>0.80836210116971</t>
+    <t>0.808241125316453</t>
+  </si>
+  <si>
+    <t>0.794148033714476</t>
+  </si>
+  <si>
+    <t>0.822334216918429</t>
   </si>
   <si>
     <t>Access to healthcare</t>
@@ -530,394 +530,394 @@
     <t>% of HH spending more than 20% of total expenditure on healthcare</t>
   </si>
   <si>
-    <t>0.123128712105339</t>
-  </si>
-  <si>
-    <t>0.108525580447503</t>
-  </si>
-  <si>
-    <t>0.137731843763176</t>
-  </si>
-  <si>
-    <t>0.789479800364062</t>
-  </si>
-  <si>
-    <t>0.768336955745277</t>
-  </si>
-  <si>
-    <t>0.810622644982847</t>
-  </si>
-  <si>
-    <t>1.70328645342669</t>
-  </si>
-  <si>
-    <t>1.68114048351008</t>
-  </si>
-  <si>
-    <t>1.72543242334329</t>
-  </si>
-  <si>
-    <t>0.00281322525440915</t>
-  </si>
-  <si>
-    <t>0.00112987197623113</t>
-  </si>
-  <si>
-    <t>0.00449657853258717</t>
-  </si>
-  <si>
-    <t>0.707092878801738</t>
-  </si>
-  <si>
-    <t>0.688400480858055</t>
-  </si>
-  <si>
-    <t>0.725785276745421</t>
-  </si>
-  <si>
-    <t>0.773766357756652</t>
-  </si>
-  <si>
-    <t>0.756595269075077</t>
-  </si>
-  <si>
-    <t>0.790937446438227</t>
-  </si>
-  <si>
-    <t>0.0429208706778323</t>
-  </si>
-  <si>
-    <t>0.0348709112436895</t>
-  </si>
-  <si>
-    <t>0.0509708301119751</t>
-  </si>
-  <si>
-    <t>0.247136919263199</t>
-  </si>
-  <si>
-    <t>0.229678730743415</t>
-  </si>
-  <si>
-    <t>0.264595107782983</t>
-  </si>
-  <si>
-    <t>0.131173010494393</t>
-  </si>
-  <si>
-    <t>0.112541616339381</t>
-  </si>
-  <si>
-    <t>0.149804404649405</t>
-  </si>
-  <si>
-    <t>0.894754564949322</t>
-  </si>
-  <si>
-    <t>0.838101888938598</t>
-  </si>
-  <si>
-    <t>0.951407240960046</t>
-  </si>
-  <si>
-    <t>0.214652539622201</t>
-  </si>
-  <si>
-    <t>0.199027398242183</t>
-  </si>
-  <si>
-    <t>0.230277681002219</t>
-  </si>
-  <si>
-    <t>0.599497996284062</t>
-  </si>
-  <si>
-    <t>0.57280091137073</t>
-  </si>
-  <si>
-    <t>0.626195081197395</t>
-  </si>
-  <si>
-    <t>0.431341405678296</t>
-  </si>
-  <si>
-    <t>0.41039084547319</t>
-  </si>
-  <si>
-    <t>0.452291965883401</t>
-  </si>
-  <si>
-    <t>0.654621789613537</t>
-  </si>
-  <si>
-    <t>0.635396535524669</t>
-  </si>
-  <si>
-    <t>0.673847043702405</t>
-  </si>
-  <si>
-    <t>0.921166255831698</t>
-  </si>
-  <si>
-    <t>0.911101821230267</t>
-  </si>
-  <si>
-    <t>0.931230690433129</t>
-  </si>
-  <si>
-    <t>0.790997770439237</t>
-  </si>
-  <si>
-    <t>0.773547416366404</t>
-  </si>
-  <si>
-    <t>0.80844812451207</t>
-  </si>
-  <si>
-    <t>0.0154750502452402</t>
-  </si>
-  <si>
-    <t>0.0109716863950981</t>
-  </si>
-  <si>
-    <t>0.0199784140953824</t>
-  </si>
-  <si>
-    <t>0.17478861818865</t>
-  </si>
-  <si>
-    <t>0.158139569432192</t>
-  </si>
-  <si>
-    <t>0.191437666945109</t>
-  </si>
-  <si>
-    <t>0.0137114154887288</t>
-  </si>
-  <si>
-    <t>0.00933117937756459</t>
-  </si>
-  <si>
-    <t>0.0180916515998929</t>
+    <t>0.124976143849311</t>
+  </si>
+  <si>
+    <t>0.112613801716461</t>
+  </si>
+  <si>
+    <t>0.137338485982162</t>
+  </si>
+  <si>
+    <t>0.752394403834651</t>
+  </si>
+  <si>
+    <t>0.726846148998199</t>
+  </si>
+  <si>
+    <t>0.777942658671103</t>
+  </si>
+  <si>
+    <t>1.68804443287072</t>
+  </si>
+  <si>
+    <t>1.66054478196138</t>
+  </si>
+  <si>
+    <t>1.71554408378007</t>
+  </si>
+  <si>
+    <t>0.00472565178762906</t>
+  </si>
+  <si>
+    <t>0.00101190450672168</t>
+  </si>
+  <si>
+    <t>0.00843939906853643</t>
+  </si>
+  <si>
+    <t>0.73708906204081</t>
+  </si>
+  <si>
+    <t>0.718459991591604</t>
+  </si>
+  <si>
+    <t>0.755718132490016</t>
+  </si>
+  <si>
+    <t>0.726362118714024</t>
+  </si>
+  <si>
+    <t>0.706352282871395</t>
+  </si>
+  <si>
+    <t>0.746371954556652</t>
+  </si>
+  <si>
+    <t>0.0523483653822304</t>
+  </si>
+  <si>
+    <t>0.0437222656064363</t>
+  </si>
+  <si>
+    <t>0.0609744651580245</t>
+  </si>
+  <si>
+    <t>0.271145213869855</t>
+  </si>
+  <si>
+    <t>0.25200562157212</t>
+  </si>
+  <si>
+    <t>0.29028480616759</t>
+  </si>
+  <si>
+    <t>0.102525720841312</t>
+  </si>
+  <si>
+    <t>0.0874927019729855</t>
+  </si>
+  <si>
+    <t>0.117558739709639</t>
+  </si>
+  <si>
+    <t>0.75462286705146</t>
+  </si>
+  <si>
+    <t>0.632738628506707</t>
+  </si>
+  <si>
+    <t>0.876507105596213</t>
+  </si>
+  <si>
+    <t>0.196647713195493</t>
+  </si>
+  <si>
+    <t>0.183011399232788</t>
+  </si>
+  <si>
+    <t>0.210284027158198</t>
+  </si>
+  <si>
+    <t>0.579338770772205</t>
+  </si>
+  <si>
+    <t>0.550872329586068</t>
+  </si>
+  <si>
+    <t>0.607805211958342</t>
+  </si>
+  <si>
+    <t>0.444194276228374</t>
+  </si>
+  <si>
+    <t>0.422372491266222</t>
+  </si>
+  <si>
+    <t>0.466016061190527</t>
+  </si>
+  <si>
+    <t>0.69231859613052</t>
+  </si>
+  <si>
+    <t>0.672673482934418</t>
+  </si>
+  <si>
+    <t>0.711963709326621</t>
+  </si>
+  <si>
+    <t>0.937488383730074</t>
+  </si>
+  <si>
+    <t>0.928637990162592</t>
+  </si>
+  <si>
+    <t>0.946338777297555</t>
+  </si>
+  <si>
+    <t>0.747054724219356</t>
+  </si>
+  <si>
+    <t>0.725340804682053</t>
+  </si>
+  <si>
+    <t>0.76876864375666</t>
+  </si>
+  <si>
+    <t>0.0103745214916886</t>
+  </si>
+  <si>
+    <t>0.00715241125342056</t>
+  </si>
+  <si>
+    <t>0.0135966317299567</t>
+  </si>
+  <si>
+    <t>0.222338412957222</t>
+  </si>
+  <si>
+    <t>0.201027496303062</t>
+  </si>
+  <si>
+    <t>0.243649329611382</t>
+  </si>
+  <si>
+    <t>0.0160265823683038</t>
+  </si>
+  <si>
+    <t>0.0102521697096422</t>
+  </si>
+  <si>
+    <t>0.0218009950269654</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>0.740062093132674</t>
-  </si>
-  <si>
-    <t>0.72225464502424</t>
-  </si>
-  <si>
-    <t>0.757869541241108</t>
-  </si>
-  <si>
-    <t>0.239750417031294</t>
-  </si>
-  <si>
-    <t>0.221803670584166</t>
-  </si>
-  <si>
-    <t>0.257697163478422</t>
-  </si>
-  <si>
-    <t>0.715148999648262</t>
-  </si>
-  <si>
-    <t>0.687241079535804</t>
-  </si>
-  <si>
-    <t>0.743056919760721</t>
-  </si>
-  <si>
-    <t>1.59628193281508</t>
-  </si>
-  <si>
-    <t>1.56214449818524</t>
-  </si>
-  <si>
-    <t>1.63041936744493</t>
-  </si>
-  <si>
-    <t>0.0173233771061183</t>
-  </si>
-  <si>
-    <t>0.0122228801690698</t>
-  </si>
-  <si>
-    <t>0.0224238740431668</t>
-  </si>
-  <si>
-    <t>0.756380509363109</t>
-  </si>
-  <si>
-    <t>0.733646394600408</t>
-  </si>
-  <si>
-    <t>0.779114624125811</t>
-  </si>
-  <si>
-    <t>0.53980975330524</t>
-  </si>
-  <si>
-    <t>0.511916320899922</t>
-  </si>
-  <si>
-    <t>0.567703185710558</t>
-  </si>
-  <si>
-    <t>0.166127817261124</t>
-  </si>
-  <si>
-    <t>0.142146538583475</t>
-  </si>
-  <si>
-    <t>0.190109095938774</t>
-  </si>
-  <si>
-    <t>0.35699458853235</t>
-  </si>
-  <si>
-    <t>0.329772967118371</t>
-  </si>
-  <si>
-    <t>0.384216209946329</t>
-  </si>
-  <si>
-    <t>0.0943212603642976</t>
-  </si>
-  <si>
-    <t>0.0751943994706085</t>
-  </si>
-  <si>
-    <t>0.113448121257987</t>
-  </si>
-  <si>
-    <t>0.830311271748416</t>
-  </si>
-  <si>
-    <t>0.725958753424895</t>
-  </si>
-  <si>
-    <t>0.934663790071937</t>
-  </si>
-  <si>
-    <t>0.00740510275399231</t>
-  </si>
-  <si>
-    <t>0.00237742268151377</t>
-  </si>
-  <si>
-    <t>0.0124327828264709</t>
-  </si>
-  <si>
-    <t>0.610801351742174</t>
-  </si>
-  <si>
-    <t>0.579251829363166</t>
-  </si>
-  <si>
-    <t>0.642350874121181</t>
-  </si>
-  <si>
-    <t>0.0716459816063685</t>
-  </si>
-  <si>
-    <t>0.0558499048125132</t>
-  </si>
-  <si>
-    <t>0.0874420584002238</t>
-  </si>
-  <si>
-    <t>0.607349623506624</t>
-  </si>
-  <si>
-    <t>0.580935861650209</t>
-  </si>
-  <si>
-    <t>0.633763385363039</t>
-  </si>
-  <si>
-    <t>0.660665010130207</t>
-  </si>
-  <si>
-    <t>0.634958797827992</t>
-  </si>
-  <si>
-    <t>0.686371222432422</t>
-  </si>
-  <si>
-    <t>0.0382231311804104</t>
-  </si>
-  <si>
-    <t>0.0260444300372091</t>
-  </si>
-  <si>
-    <t>0.0504018323236116</t>
-  </si>
-  <si>
-    <t>0.0457090163363796</t>
-  </si>
-  <si>
-    <t>0.0337492459625129</t>
-  </si>
-  <si>
-    <t>0.0576687867102463</t>
-  </si>
-  <si>
-    <t>0.86905015814978</t>
-  </si>
-  <si>
-    <t>0.799867818424943</t>
-  </si>
-  <si>
-    <t>0.938232497874618</t>
-  </si>
-  <si>
-    <t>0.0487602449128395</t>
-  </si>
-  <si>
-    <t>0.00685440387835692</t>
-  </si>
-  <si>
-    <t>0.0906660859473221</t>
-  </si>
-  <si>
-    <t>0.0684437959556856</t>
-  </si>
-  <si>
-    <t>0.0152798458196504</t>
-  </si>
-  <si>
-    <t>0.121607746091721</t>
-  </si>
-  <si>
-    <t>0.011760293778483</t>
-  </si>
-  <si>
-    <t>-0.0017699565563314</t>
-  </si>
-  <si>
-    <t>0.0252905441132973</t>
-  </si>
-  <si>
-    <t>0.778225494942676</t>
-  </si>
-  <si>
-    <t>0.756075871930285</t>
-  </si>
-  <si>
-    <t>0.800375117955067</t>
-  </si>
-  <si>
-    <t>0.133997154026202</t>
-  </si>
-  <si>
-    <t>0.116031728081232</t>
-  </si>
-  <si>
-    <t>0.151962579971172</t>
+    <t>0.791127666068691</t>
+  </si>
+  <si>
+    <t>0.775183723987242</t>
+  </si>
+  <si>
+    <t>0.80707160815014</t>
+  </si>
+  <si>
+    <t>0.283660953667286</t>
+  </si>
+  <si>
+    <t>0.263831540659856</t>
+  </si>
+  <si>
+    <t>0.303490366674716</t>
+  </si>
+  <si>
+    <t>0.708279290187398</t>
+  </si>
+  <si>
+    <t>0.684413959788025</t>
+  </si>
+  <si>
+    <t>0.732144620586771</t>
+  </si>
+  <si>
+    <t>1.58508029786159</t>
+  </si>
+  <si>
+    <t>1.55117328784653</t>
+  </si>
+  <si>
+    <t>1.61898730787665</t>
+  </si>
+  <si>
+    <t>0.0166224869150339</t>
+  </si>
+  <si>
+    <t>0.0124313983705175</t>
+  </si>
+  <si>
+    <t>0.0208135754595503</t>
+  </si>
+  <si>
+    <t>0.752276630373103</t>
+  </si>
+  <si>
+    <t>0.732767262498352</t>
+  </si>
+  <si>
+    <t>0.771785998247855</t>
+  </si>
+  <si>
+    <t>0.528813636518097</t>
+  </si>
+  <si>
+    <t>0.505252305361256</t>
+  </si>
+  <si>
+    <t>0.552374967674938</t>
+  </si>
+  <si>
+    <t>0.16061251574495</t>
+  </si>
+  <si>
+    <t>0.140873297977079</t>
+  </si>
+  <si>
+    <t>0.180351733512821</t>
+  </si>
+  <si>
+    <t>0.357040691554403</t>
+  </si>
+  <si>
+    <t>0.334118640392503</t>
+  </si>
+  <si>
+    <t>0.379962742716302</t>
+  </si>
+  <si>
+    <t>0.0900335455605125</t>
+  </si>
+  <si>
+    <t>0.0743761344829881</t>
+  </si>
+  <si>
+    <t>0.105690956638037</t>
+  </si>
+  <si>
+    <t>0.79447083184937</t>
+  </si>
+  <si>
+    <t>0.687734995672173</t>
+  </si>
+  <si>
+    <t>0.901206668026567</t>
+  </si>
+  <si>
+    <t>0.00774832886057329</t>
+  </si>
+  <si>
+    <t>0.00352109175641441</t>
+  </si>
+  <si>
+    <t>0.0119755659647322</t>
+  </si>
+  <si>
+    <t>0.609666418821631</t>
+  </si>
+  <si>
+    <t>0.583093508027564</t>
+  </si>
+  <si>
+    <t>0.636239329615698</t>
+  </si>
+  <si>
+    <t>0.0710088497882305</t>
+  </si>
+  <si>
+    <t>0.0579088845452661</t>
+  </si>
+  <si>
+    <t>0.0841088150311948</t>
+  </si>
+  <si>
+    <t>0.601903835824463</t>
+  </si>
+  <si>
+    <t>0.579482888867684</t>
+  </si>
+  <si>
+    <t>0.624324782781242</t>
+  </si>
+  <si>
+    <t>0.660071559437788</t>
+  </si>
+  <si>
+    <t>0.63833507861533</t>
+  </si>
+  <si>
+    <t>0.681808040260246</t>
+  </si>
+  <si>
+    <t>0.0382034891637169</t>
+  </si>
+  <si>
+    <t>0.0282057509569678</t>
+  </si>
+  <si>
+    <t>0.048201227370466</t>
+  </si>
+  <si>
+    <t>0.0428145573993657</t>
+  </si>
+  <si>
+    <t>0.033324563342043</t>
+  </si>
+  <si>
+    <t>0.0523045514566885</t>
+  </si>
+  <si>
+    <t>0.870551200645308</t>
+  </si>
+  <si>
+    <t>0.812316148130295</t>
+  </si>
+  <si>
+    <t>0.928786253160321</t>
+  </si>
+  <si>
+    <t>0.050176613986501</t>
+  </si>
+  <si>
+    <t>0.013624456173878</t>
+  </si>
+  <si>
+    <t>0.086728771799124</t>
+  </si>
+  <si>
+    <t>0.0663819837150296</t>
+  </si>
+  <si>
+    <t>0.0224007907647354</t>
+  </si>
+  <si>
+    <t>0.110363176665324</t>
+  </si>
+  <si>
+    <t>0.0109376295583821</t>
+  </si>
+  <si>
+    <t>0.000365562348675647</t>
+  </si>
+  <si>
+    <t>0.0215096967680886</t>
+  </si>
+  <si>
+    <t>0.774008243801387</t>
+  </si>
+  <si>
+    <t>0.754935925757654</t>
+  </si>
+  <si>
+    <t>0.793080561845119</t>
+  </si>
+  <si>
+    <t>0.133567089058128</t>
+  </si>
+  <si>
+    <t>0.118362625768159</t>
+  </si>
+  <si>
+    <t>0.148771552348097</t>
   </si>
 </sst>
 </file>

</xml_diff>